<commit_message>
SQLDatabase ready, datainfo almostready
</commit_message>
<xml_diff>
--- a/Santa's Toy Factory1.xlsx
+++ b/Santa's Toy Factory1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Products-MongoDB" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="186">
   <si>
     <t>Column Names</t>
   </si>
@@ -430,13 +430,163 @@
   </si>
   <si>
     <t xml:space="preserve">Gift value Grouped by Age and By Toy Type </t>
+  </si>
+  <si>
+    <t>GROUPAGE</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Infant - Just born </t>
+  </si>
+  <si>
+    <t>Baby - Hasn't been alive for long </t>
+  </si>
+  <si>
+    <t>Toddler - 1-2-3 yrs </t>
+  </si>
+  <si>
+    <t>Child - 3-12 years old </t>
+  </si>
+  <si>
+    <t>Teen - 13-19 years old </t>
+  </si>
+  <si>
+    <t>Adult - 20-55 years old </t>
+  </si>
+  <si>
+    <t>Senior - 55-80 </t>
+  </si>
+  <si>
+    <t>Golden Oldie - 80 and above</t>
+  </si>
+  <si>
+    <t>TOYS</t>
+  </si>
+  <si>
+    <t>Bratz</t>
+  </si>
+  <si>
+    <t>fashion doll</t>
+  </si>
+  <si>
+    <t>Mindflex</t>
+  </si>
+  <si>
+    <t>Using advanced technology, a wireless EEG headset reads your brainwave activity and uses it to guide a blue Mindflex ball through a series of obstacles</t>
+  </si>
+  <si>
+    <t>Zhu Zhu</t>
+  </si>
+  <si>
+    <t>robotic hamsters</t>
+  </si>
+  <si>
+    <t>Neodymium-Magnet Toy</t>
+  </si>
+  <si>
+    <t>rare-earth magnets </t>
+  </si>
+  <si>
+    <t>Furby</t>
+  </si>
+  <si>
+    <t>ech-toy market</t>
+  </si>
+  <si>
+    <t>Tickle Me Elmo</t>
+  </si>
+  <si>
+    <t>stuffed animal that would laugh when tickled by its owner</t>
+  </si>
+  <si>
+    <t>American Girl Doll</t>
+  </si>
+  <si>
+    <t>dolls' realistic personalities, modeled after ordinary girls from American history and modern times</t>
+  </si>
+  <si>
+    <t>Buzz Lightyear</t>
+  </si>
+  <si>
+    <t>futuristic astronaut with an appreciation for gadgets and a zest for intergalactic travel</t>
+  </si>
+  <si>
+    <t>Beanie Baby</t>
+  </si>
+  <si>
+    <t>mall-scale stuffed animals filled with tiny plastic beads to give them a sturdy but flexible feel</t>
+  </si>
+  <si>
+    <t>Super Soaker</t>
+  </si>
+  <si>
+    <t>gun that's able to fire water a distance of up to 50 ft.</t>
+  </si>
+  <si>
+    <t>Little Tikes Cozy Coupe Car</t>
+  </si>
+  <si>
+    <t>classic red-and-yellow car</t>
+  </si>
+  <si>
+    <t>Little Tikes Log Cabin</t>
+  </si>
+  <si>
+    <t>playhouse</t>
+  </si>
+  <si>
+    <t>Wrestling Buddy</t>
+  </si>
+  <si>
+    <t>pillow in the shape of an elite pro-wrestling personality</t>
+  </si>
+  <si>
+    <t>Glow Stick</t>
+  </si>
+  <si>
+    <t>government or military emergencies after dark. glow sticks were adopted by kids who were going camping or trick-or-treating</t>
+  </si>
+  <si>
+    <t>Skip-It</t>
+  </si>
+  <si>
+    <t> small ankle hoop with attached ball and chain that kept track of its rotations</t>
+  </si>
+  <si>
+    <t>Teenage Mutant Ninja Turtles</t>
+  </si>
+  <si>
+    <t>superheroes</t>
+  </si>
+  <si>
+    <t>Koosh Ball</t>
+  </si>
+  <si>
+    <t>A ball made out of rubber fibers that were easily grabbed by tiny fingers</t>
+  </si>
+  <si>
+    <t>Pound Puppy</t>
+  </si>
+  <si>
+    <t>Snoopy Sno-Cone Machine</t>
+  </si>
+  <si>
+    <t>Teddy Ruxpin</t>
+  </si>
+  <si>
+    <t>stuffed animal used cassette tapes to "read" to its young companions</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,6 +617,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -482,7 +670,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -631,48 +819,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
@@ -738,10 +889,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Нормален" xfId="0" builtinId="0"/>
@@ -1365,293 +1523,290 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H112"/>
+  <dimension ref="A3:I156"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="I97" sqref="I97"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="K146" sqref="K146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>128</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>2</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>2</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>15</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>0</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>2</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>3</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>14</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>0</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>5</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>27</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>1</v>
-      </c>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
         <v>11</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>2</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
         <v>28</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>3</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>0</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>5</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>1</v>
-      </c>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
         <v>11</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>2</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>3</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>0</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>5</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>44</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>35</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>45</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>1</v>
-      </c>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
         <v>46</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>47</v>
-      </c>
-      <c r="D34" t="s">
-        <v>11</v>
       </c>
       <c r="E34" t="s">
         <v>11</v>
@@ -1659,824 +1814,1142 @@
       <c r="F34" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="G34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>2</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" s="14">
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" s="14">
         <v>41922</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>100</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>2</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>3</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>15</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>1</v>
-      </c>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
         <v>5</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>6</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>62</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>65</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
         <v>2</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>11</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>12</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>2011</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>67</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>3</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>68</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="22" t="s">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="B47" s="16" t="s">
+      <c r="C47" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="D47" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="16" t="s">
+      <c r="E47" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E47" s="16" t="s">
+      <c r="F47" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="F47" s="17" t="s">
+      <c r="G47" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="G47" s="33"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="18" t="s">
+      <c r="H47" s="33"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B48" s="19">
-        <v>1</v>
-      </c>
-      <c r="C48" s="19" t="s">
+      <c r="C48" s="19">
+        <v>1</v>
+      </c>
+      <c r="D48" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D48" s="19">
+      <c r="E48" s="19">
         <v>120</v>
       </c>
-      <c r="E48" s="19" t="s">
+      <c r="F48" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="F48" s="20">
-        <v>1</v>
-      </c>
-      <c r="G48" s="20"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="21"/>
+      <c r="G48" s="20">
+        <v>1</v>
+      </c>
+      <c r="H48" s="20"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="21"/>
       <c r="C49" s="21"/>
       <c r="D49" s="21"/>
       <c r="E49" s="21"/>
       <c r="F49" s="21"/>
       <c r="G49" s="21"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="22" t="s">
+      <c r="H49" s="21"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="B50" s="16" t="s">
+      <c r="C50" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C50" s="16" t="s">
+      <c r="D50" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D50" s="17" t="s">
+      <c r="E50" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E50" s="39" t="s">
+      <c r="F50" s="33" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="27" t="s">
+    <row r="51" spans="2:8" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="B51" s="28">
-        <v>1</v>
-      </c>
-      <c r="C51" s="28" t="s">
+      <c r="C51" s="28">
+        <v>1</v>
+      </c>
+      <c r="D51" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="D51" s="29" t="s">
+      <c r="E51" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="E51" s="40" t="s">
+      <c r="F51" s="29" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="27" t="s">
+    <row r="52" spans="2:8" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="B52" s="28">
+      <c r="C52" s="28">
         <v>2</v>
       </c>
-      <c r="C52" s="28" t="s">
+      <c r="D52" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="D52" s="29" t="s">
+      <c r="E52" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="E52" s="40" t="s">
+      <c r="F52" s="29" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="27" t="s">
+    <row r="53" spans="2:8" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B53" s="37">
+      <c r="C53" s="37">
         <v>3</v>
       </c>
-      <c r="C53" s="28" t="s">
+      <c r="D53" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="D53" s="29" t="s">
+      <c r="E53" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="E53" s="40" t="s">
+      <c r="F53" s="29" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="27" t="s">
+    <row r="54" spans="2:8" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="B54" s="37">
+      <c r="C54" s="37">
         <v>4</v>
       </c>
-      <c r="C54" s="28" t="s">
+      <c r="D54" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="D54" s="29" t="s">
+      <c r="E54" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="E54" s="40" t="s">
+      <c r="F54" s="29" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="27" t="s">
+    <row r="55" spans="2:8" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="B55" s="37">
+      <c r="C55" s="37">
         <v>5</v>
       </c>
-      <c r="C55" s="28" t="s">
+      <c r="D55" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="D55" s="29" t="s">
+      <c r="E55" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="E55" s="40" t="s">
+      <c r="F55" s="29" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="18"/>
-      <c r="B56" s="19"/>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="18"/>
       <c r="C56" s="19"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="41"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="22" t="s">
+      <c r="D56" s="19"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="20"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="B58" s="16" t="s">
+      <c r="C58" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C58" s="16" t="s">
+      <c r="D58" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="D58" s="17" t="s">
+      <c r="E58" s="17" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="27" t="s">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B59" s="21">
-        <v>1</v>
-      </c>
-      <c r="C59" s="27" t="s">
+      <c r="C59" s="21">
+        <v>1</v>
+      </c>
+      <c r="D59" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="D59" s="35" t="s">
+      <c r="E59" s="35" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="27" t="s">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="B60" s="21">
+      <c r="C60" s="21">
         <v>2</v>
       </c>
-      <c r="C60" s="27" t="s">
+      <c r="D60" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="D60" s="35" t="s">
+      <c r="E60" s="35" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="27" t="s">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="B61" s="21">
+      <c r="C61" s="21">
         <v>3</v>
       </c>
-      <c r="C61" s="27" t="s">
+      <c r="D61" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="D61" s="35" t="s">
+      <c r="E61" s="35" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="27" t="s">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="B62" s="23">
+      <c r="C62" s="23">
         <v>4</v>
       </c>
-      <c r="C62" s="27" t="s">
+      <c r="D62" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="D62" s="35" t="s">
+      <c r="E62" s="35" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="27" t="s">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="B63" s="23">
+      <c r="C63" s="23">
         <v>5</v>
       </c>
-      <c r="C63" s="27" t="s">
+      <c r="D63" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="D63" s="35" t="s">
+      <c r="E63" s="35" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="27" t="s">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="B64" s="23">
+      <c r="C64" s="23">
         <v>6</v>
       </c>
-      <c r="C64" s="27" t="s">
+      <c r="D64" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="D64" s="35" t="s">
+      <c r="E64" s="35" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="18"/>
-      <c r="B65" s="19"/>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="18"/>
       <c r="C65" s="19"/>
-      <c r="D65" s="20"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="22" t="s">
+      <c r="D65" s="19"/>
+      <c r="E65" s="20"/>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="B67" s="16" t="s">
+      <c r="C67" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C67" s="16" t="s">
+      <c r="D67" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D67" s="17" t="s">
+      <c r="E67" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="E67" s="21"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="18" t="s">
+      <c r="F67" s="21"/>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B68" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="B68" s="19">
-        <v>1</v>
-      </c>
-      <c r="C68" s="19" t="s">
+      <c r="C68" s="19">
+        <v>1</v>
+      </c>
+      <c r="D68" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="D68" s="20" t="s">
+      <c r="E68" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="E68" s="21"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="22" t="s">
+      <c r="F68" s="21"/>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="B70" s="16" t="s">
+      <c r="C70" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C70" s="16" t="s">
+      <c r="D70" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D70" s="16" t="s">
+      <c r="E70" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="E70" s="17" t="s">
+      <c r="F70" s="17" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="18" t="s">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="B71" s="19">
-        <v>1</v>
-      </c>
-      <c r="C71" s="19" t="s">
+      <c r="C71" s="19">
+        <v>1</v>
+      </c>
+      <c r="D71" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="D71" s="19" t="s">
+      <c r="E71" s="19">
+        <v>1</v>
+      </c>
+      <c r="F71" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="E71" s="20" t="s">
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B73" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="C73" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D73" s="17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B74" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C74" s="21">
+        <v>1</v>
+      </c>
+      <c r="D74" s="35" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B75" s="24"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="35"/>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B76" s="24"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="35"/>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B77" s="24"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="35"/>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B78" s="24"/>
+      <c r="C78" s="21"/>
+      <c r="D78" s="35"/>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B79" s="18"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="20"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B82" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C82" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D82" s="17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B83" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C83" s="19">
+        <v>1</v>
+      </c>
+      <c r="D83" s="20" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="B73" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="C73" s="17" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="B74" s="21">
-        <v>1</v>
-      </c>
-      <c r="C74" s="35" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="24"/>
-      <c r="B75" s="21"/>
-      <c r="C75" s="35"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="24"/>
-      <c r="B76" s="21"/>
-      <c r="C76" s="35"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="24"/>
-      <c r="B77" s="21"/>
-      <c r="C77" s="35"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="24"/>
-      <c r="B78" s="21"/>
-      <c r="C78" s="35"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="18"/>
-      <c r="B79" s="19"/>
-      <c r="C79" s="20"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="B82" s="16" t="s">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B85" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C85" s="25"/>
+      <c r="D85" s="26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B86" s="27"/>
+      <c r="C86" s="28">
+        <v>1</v>
+      </c>
+      <c r="D86" s="29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B87" s="30"/>
+      <c r="C87" s="31">
+        <v>2</v>
+      </c>
+      <c r="D87" s="32" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B89" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C89" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C82" s="17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="B83" s="19">
-        <v>1</v>
-      </c>
-      <c r="C83" s="20" t="s">
+      <c r="D89" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E89" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F89" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G89" s="17"/>
+      <c r="H89" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B90" s="24"/>
+      <c r="C90" s="21">
+        <v>1</v>
+      </c>
+      <c r="D90" s="21">
+        <v>1999</v>
+      </c>
+      <c r="E90" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="F90" s="21" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="B85" s="25"/>
-      <c r="C85" s="26" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="27"/>
-      <c r="B86" s="28">
-        <v>1</v>
-      </c>
-      <c r="C86" s="29" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="30"/>
-      <c r="B87" s="31">
+      <c r="G90" s="35"/>
+      <c r="H90" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="I90" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B91" s="24"/>
+      <c r="C91" s="23">
         <v>2</v>
       </c>
-      <c r="C87" s="32" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="B89" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C89" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D89" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E89" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="F89" s="17"/>
-      <c r="G89" s="16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="24"/>
-      <c r="B90" s="21">
-        <v>1</v>
-      </c>
-      <c r="C90" s="21">
-        <v>1999</v>
-      </c>
-      <c r="D90" s="21" t="s">
+      <c r="D91" s="21">
+        <v>2000</v>
+      </c>
+      <c r="E91" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="E90" s="21" t="s">
+      <c r="F91" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="F90" s="35"/>
-      <c r="G90" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="H90" s="23" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="24"/>
-      <c r="B91" s="23">
-        <v>2</v>
-      </c>
-      <c r="C91" s="21">
-        <v>2000</v>
-      </c>
-      <c r="D91" s="21" t="s">
+      <c r="G91" s="35"/>
+      <c r="H91" s="23"/>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B92" s="24"/>
+      <c r="C92" s="21">
+        <v>3</v>
+      </c>
+      <c r="D92" s="21">
+        <v>2001</v>
+      </c>
+      <c r="E92" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="E91" s="21" t="s">
+      <c r="F92" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="F91" s="35"/>
-      <c r="G91" s="23"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="24"/>
-      <c r="B92" s="21">
-        <v>3</v>
-      </c>
-      <c r="C92" s="21">
-        <v>2001</v>
-      </c>
-      <c r="D92" s="21" t="s">
+      <c r="G92" s="35"/>
+      <c r="H92" s="23"/>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B93" s="24"/>
+      <c r="C93" s="23">
+        <v>4</v>
+      </c>
+      <c r="D93" s="21">
+        <v>2002</v>
+      </c>
+      <c r="E93" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="E92" s="21" t="s">
+      <c r="F93" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="F92" s="35"/>
-      <c r="G92" s="23"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="24"/>
-      <c r="B93" s="23">
-        <v>4</v>
-      </c>
-      <c r="C93" s="21">
-        <v>2002</v>
-      </c>
-      <c r="D93" s="21" t="s">
+      <c r="G93" s="35"/>
+      <c r="H93" s="23"/>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B94" s="24"/>
+      <c r="C94" s="21">
+        <v>5</v>
+      </c>
+      <c r="D94" s="21">
+        <v>2003</v>
+      </c>
+      <c r="E94" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="E93" s="21" t="s">
+      <c r="F94" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="F93" s="35"/>
-      <c r="G93" s="23"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="24"/>
-      <c r="B94" s="21">
-        <v>5</v>
-      </c>
-      <c r="C94" s="21">
-        <v>2003</v>
-      </c>
-      <c r="D94" s="21" t="s">
+      <c r="G94" s="35"/>
+      <c r="H94" s="23"/>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B95" s="18"/>
+      <c r="C95" s="38">
+        <v>6</v>
+      </c>
+      <c r="D95" s="19">
+        <v>2004</v>
+      </c>
+      <c r="E95" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="E94" s="21" t="s">
+      <c r="F95" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="F94" s="35"/>
-      <c r="G94" s="23"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="18"/>
-      <c r="B95" s="38">
-        <v>6</v>
-      </c>
-      <c r="C95" s="19">
-        <v>2004</v>
-      </c>
-      <c r="D95" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="E95" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="F95" s="20"/>
-      <c r="G95" s="21"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="21"/>
-      <c r="B96" s="23"/>
-      <c r="C96" s="21"/>
+      <c r="G95" s="20"/>
+      <c r="H95" s="21"/>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B96" s="21"/>
+      <c r="C96" s="23"/>
       <c r="D96" s="21"/>
       <c r="E96" s="21"/>
       <c r="F96" s="21"/>
       <c r="G96" s="21"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="15" t="s">
+      <c r="H96" s="21"/>
+    </row>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B97" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B97" s="42" t="s">
+      <c r="C97" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="C97" s="16" t="s">
+      <c r="D97" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="D97" s="42" t="s">
+      <c r="E97" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="E97" s="33" t="s">
+      <c r="F97" s="33" t="s">
         <v>130</v>
       </c>
-      <c r="F97" s="21"/>
       <c r="G97" s="21"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="34"/>
-      <c r="B98" s="23">
-        <v>1</v>
-      </c>
+      <c r="H97" s="21"/>
+    </row>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B98" s="34"/>
       <c r="C98" s="23">
+        <v>1</v>
+      </c>
+      <c r="D98" s="23">
         <v>100</v>
       </c>
-      <c r="D98" s="21">
-        <v>1</v>
-      </c>
-      <c r="E98" s="35">
-        <v>1</v>
-      </c>
-      <c r="F98" s="21"/>
+      <c r="E98" s="21">
+        <v>1</v>
+      </c>
+      <c r="F98" s="35">
+        <v>1</v>
+      </c>
       <c r="G98" s="21"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="34"/>
-      <c r="B99" s="23">
+      <c r="H98" s="21"/>
+    </row>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B99" s="34"/>
+      <c r="C99" s="23">
         <v>2</v>
       </c>
-      <c r="C99" s="23">
+      <c r="D99" s="23">
         <v>50</v>
       </c>
-      <c r="D99" s="21"/>
-      <c r="E99" s="35"/>
-      <c r="F99" s="21"/>
+      <c r="E99" s="21"/>
+      <c r="F99" s="35"/>
       <c r="G99" s="21"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="18"/>
-      <c r="B100" s="38"/>
-      <c r="C100" s="19"/>
+      <c r="H99" s="21"/>
+    </row>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B100" s="18"/>
+      <c r="C100" s="38"/>
       <c r="D100" s="19"/>
-      <c r="E100" s="20"/>
-      <c r="F100" s="21"/>
+      <c r="E100" s="19"/>
+      <c r="F100" s="20"/>
       <c r="G100" s="21"/>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="22" t="s">
+      <c r="H100" s="21"/>
+    </row>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B102" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="B102" s="16" t="s">
+      <c r="C102" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C102" s="16" t="s">
+      <c r="D102" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D102" s="16" t="s">
+      <c r="E102" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="E102" s="16" t="s">
+      <c r="F102" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="F102" s="16" t="s">
+      <c r="G102" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="G102" s="17" t="s">
+      <c r="H102" s="17" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="18" t="s">
+    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B103" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="B103" s="19">
-        <v>1</v>
-      </c>
-      <c r="C103" s="19" t="s">
+      <c r="C103" s="19">
+        <v>1</v>
+      </c>
+      <c r="D103" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="D103" s="19">
+      <c r="E103" s="19">
         <v>15</v>
       </c>
-      <c r="E103" s="19" t="s">
+      <c r="F103" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="F103" s="19">
-        <v>1</v>
-      </c>
-      <c r="G103" s="20"/>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="22" t="s">
+      <c r="G103" s="19">
+        <v>1</v>
+      </c>
+      <c r="H103" s="20"/>
+    </row>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B105" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="B105" s="17" t="s">
+      <c r="C105" s="17" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="34" t="s">
+      <c r="D105" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B106" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="B106" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="34" t="s">
+      <c r="C106" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B107" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="B107" s="35">
+      <c r="C107" s="35">
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="34" t="s">
+    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B108" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="B108" s="35">
+      <c r="C108" s="35">
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="34" t="s">
+    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B109" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="B109" s="35">
+      <c r="C109" s="35">
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="34" t="s">
+    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B110" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="B110" s="35">
+      <c r="C110" s="35">
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="34" t="s">
+    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B111" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="B111" s="35">
+      <c r="C111" s="35">
         <v>6</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="18" t="s">
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B112" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="B112" s="20">
+      <c r="C112" s="20">
         <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="C114" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D114" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B115" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="C115" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B116" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="C116" s="35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B117" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="C117" s="35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="41" t="s">
+        <v>141</v>
+      </c>
+      <c r="C118" s="35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B119" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C119" s="35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="41" t="s">
+        <v>143</v>
+      </c>
+      <c r="C120" s="35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="C121" s="35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="42" t="s">
+        <v>145</v>
+      </c>
+      <c r="C122" s="20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="40"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B124" s="40"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="43" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>1</v>
+      </c>
+      <c r="B126" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="C126" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="D126" s="46"/>
+    </row>
+    <row r="127" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>2</v>
+      </c>
+      <c r="B127" s="47" t="s">
+        <v>149</v>
+      </c>
+      <c r="C127" s="45" t="s">
+        <v>150</v>
+      </c>
+      <c r="D127" s="46"/>
+    </row>
+    <row r="128" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>3</v>
+      </c>
+      <c r="B128" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="C128" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="D128" s="46"/>
+    </row>
+    <row r="129" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>4</v>
+      </c>
+      <c r="B129" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="C129" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="D129" s="46"/>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>5</v>
+      </c>
+      <c r="B130" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="C130" s="44" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>6</v>
+      </c>
+      <c r="B131" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="C131" s="44" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>7</v>
+      </c>
+      <c r="B132" s="47" t="s">
+        <v>159</v>
+      </c>
+      <c r="C132" s="44" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>8</v>
+      </c>
+      <c r="B133" s="47" t="s">
+        <v>161</v>
+      </c>
+      <c r="C133" s="44" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>9</v>
+      </c>
+      <c r="B134" s="47" t="s">
+        <v>163</v>
+      </c>
+      <c r="C134" s="44" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>10</v>
+      </c>
+      <c r="B135" s="47" t="s">
+        <v>165</v>
+      </c>
+      <c r="C135" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>11</v>
+      </c>
+      <c r="B136" s="47" t="s">
+        <v>167</v>
+      </c>
+      <c r="C136" s="44" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>12</v>
+      </c>
+      <c r="B137" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="C137" s="44" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>13</v>
+      </c>
+      <c r="B138" s="47" t="s">
+        <v>171</v>
+      </c>
+      <c r="C138" s="44" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>14</v>
+      </c>
+      <c r="B139" s="47" t="s">
+        <v>173</v>
+      </c>
+      <c r="C139" s="44" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>15</v>
+      </c>
+      <c r="B140" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="C140" s="44" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>16</v>
+      </c>
+      <c r="B141" s="47" t="s">
+        <v>177</v>
+      </c>
+      <c r="C141" s="44" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>17</v>
+      </c>
+      <c r="B142" s="47" t="s">
+        <v>179</v>
+      </c>
+      <c r="C142" s="44" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>18</v>
+      </c>
+      <c r="B143" s="47" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>19</v>
+      </c>
+      <c r="B144" s="47" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>20</v>
+      </c>
+      <c r="B145" s="47" t="s">
+        <v>183</v>
+      </c>
+      <c r="C145" s="44" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B146" s="46"/>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D156" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2726,7 +3199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>

</xml_diff>